<commit_message>
created first classification model
Tested and trained on second hand made dataset of 100 images. Pretty good results but dataset was not equally spread started the making of a nice result output file
</commit_message>
<xml_diff>
--- a/code/Vision/Datasets/handmade/second_handmade/labels_new_bullet.xlsx
+++ b/code/Vision/Datasets/handmade/second_handmade/labels_new_bullet.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsdepauw/Documents/Lars.nosync/Documents/School/1Ma ing/Masterproef/TWI/code/Vision/Datasets/labels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsdepauw/Documents/Lars.nosync/Documents/School/1Ma ing/Masterproef/TWI/code/Vision/Datasets/handmade/second_handmade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B12C80B-E5FB-C247-A871-785DD4AC92D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B6E0B3-E6C4-5941-851C-08C6157C1A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{574AD3EE-55DF-7E4B-9902-E7692B0BE240}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -494,16 +494,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B54D1D-F243-824C-BA27-8F06A96566A4}">
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
     <col min="10" max="14" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -589,6 +589,9 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="G3">
+        <v>50.73</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -611,6 +614,9 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
+      <c r="G4">
+        <v>57.122</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -630,6 +636,9 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="G5">
+        <v>46.984999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -652,6 +661,9 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
+      <c r="G6">
+        <v>68.903999999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -674,6 +686,9 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
+      <c r="G7">
+        <v>35.348999999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -693,6 +708,9 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="G8">
+        <v>32.594000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -715,6 +733,9 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
+      <c r="G9">
+        <v>38.79</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -734,6 +755,9 @@
       <c r="E10">
         <v>1</v>
       </c>
+      <c r="G10">
+        <v>47.353999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -753,6 +777,9 @@
       <c r="E11">
         <v>0</v>
       </c>
+      <c r="G11">
+        <v>42.637</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -775,6 +802,9 @@
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="G12">
+        <v>44.158999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -794,6 +824,9 @@
       <c r="E13">
         <v>0</v>
       </c>
+      <c r="G13">
+        <v>40.957999999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -816,6 +849,9 @@
       <c r="F14">
         <v>1</v>
       </c>
+      <c r="G14">
+        <v>40.505000000000003</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -838,6 +874,9 @@
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="G15">
+        <v>34.71</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -857,8 +896,11 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>44.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -879,8 +921,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>75.510000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -898,8 +943,11 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>37.774999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -920,8 +968,11 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>39.883000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -939,8 +990,11 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>53.984000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -961,8 +1015,11 @@
       <c r="F21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>43.45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -980,8 +1037,11 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>51.164000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -1002,8 +1062,11 @@
       <c r="F23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>44.768999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1021,8 +1084,11 @@
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>55.622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -1043,8 +1109,11 @@
       <c r="F25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>55.427999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -1062,8 +1131,11 @@
       <c r="E26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>46.991</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -1084,8 +1156,11 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>32.549999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1103,8 +1178,11 @@
       <c r="E28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>40.301000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -1122,8 +1200,11 @@
       <c r="E29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>27.945</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -1144,8 +1225,11 @@
       <c r="F30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>31.759</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -1163,8 +1247,11 @@
       <c r="E31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>44.09</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2</v>
       </c>
@@ -1185,8 +1272,11 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>41.805</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2</v>
       </c>
@@ -1207,8 +1297,11 @@
       <c r="F33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>54.143999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -1226,8 +1319,11 @@
       <c r="E34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>42.021999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2</v>
       </c>
@@ -1245,8 +1341,11 @@
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>70.105000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -1267,8 +1366,11 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>76.501999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -1289,8 +1391,11 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>58.457000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2</v>
       </c>
@@ -1308,8 +1413,11 @@
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>72.137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -1327,8 +1435,11 @@
       <c r="E39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>108.938</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -1349,8 +1460,11 @@
       <c r="F40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>136.44200000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -1368,8 +1482,11 @@
       <c r="E41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>114.246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -1390,8 +1507,11 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>69.489999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>3</v>
       </c>
@@ -1412,8 +1532,11 @@
       <c r="F43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>157.529</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>3</v>
       </c>
@@ -1431,8 +1554,11 @@
       <c r="E44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>150.964</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -1450,8 +1576,11 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>163.71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>3</v>
       </c>
@@ -1472,8 +1601,11 @@
       <c r="F46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>250.45099999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>3</v>
       </c>
@@ -1491,8 +1623,11 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>176.70699999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>3</v>
       </c>
@@ -1513,8 +1648,11 @@
       <c r="F48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>272.12599999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -1532,8 +1670,11 @@
       <c r="E49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>159.685</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>3</v>
       </c>
@@ -1554,8 +1695,11 @@
       <c r="F50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>262.48700000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>3</v>
       </c>
@@ -1573,8 +1717,11 @@
       <c r="E51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>202.03200000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>3</v>
       </c>
@@ -1595,8 +1742,11 @@
       <c r="F52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>161.91300000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>3</v>
       </c>
@@ -1617,8 +1767,11 @@
       <c r="F53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>389.15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>3</v>
       </c>
@@ -1636,8 +1789,11 @@
       <c r="E54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>287.17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -1655,8 +1811,11 @@
       <c r="E55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>172.22200000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>3</v>
       </c>
@@ -1677,8 +1836,11 @@
       <c r="F56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>143.72300000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>3</v>
       </c>
@@ -1699,8 +1861,11 @@
       <c r="F57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>162.71199999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>3</v>
       </c>
@@ -1718,8 +1883,11 @@
       <c r="E58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>147.59100000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -1737,8 +1905,11 @@
       <c r="E59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>177.483</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>3</v>
       </c>
@@ -1759,8 +1930,11 @@
       <c r="F60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>141.84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>3</v>
       </c>
@@ -1778,8 +1952,11 @@
       <c r="E61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>168.27199999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>3</v>
       </c>
@@ -1800,8 +1977,11 @@
       <c r="F62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>164.79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>4</v>
       </c>
@@ -1819,8 +1999,11 @@
       <c r="E63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>170.90299999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>4</v>
       </c>
@@ -1841,8 +2024,11 @@
       <c r="F64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>194.83199999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>4</v>
       </c>
@@ -1860,8 +2046,11 @@
       <c r="E65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>236.77699999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>4</v>
       </c>
@@ -1882,8 +2071,11 @@
       <c r="F66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>279.31799999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>4</v>
       </c>
@@ -1904,8 +2096,11 @@
       <c r="F67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>234.07400000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>4</v>
       </c>
@@ -1923,8 +2118,11 @@
       <c r="E68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>212.64400000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>4</v>
       </c>
@@ -1942,8 +2140,11 @@
       <c r="E69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>321.149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>4</v>
       </c>
@@ -1964,8 +2165,11 @@
       <c r="F70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>226.673</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>4</v>
       </c>
@@ -1983,8 +2187,11 @@
       <c r="E71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>268.22699999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>4</v>
       </c>
@@ -2005,8 +2212,11 @@
       <c r="F72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>250.97900000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>4</v>
       </c>
@@ -2027,8 +2237,11 @@
       <c r="F73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>157.04</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>4</v>
       </c>
@@ -2046,8 +2259,11 @@
       <c r="E74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>227.3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>4</v>
       </c>
@@ -2065,8 +2281,11 @@
       <c r="E75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>180.68799999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>4</v>
       </c>
@@ -2087,8 +2306,11 @@
       <c r="F76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>192.24799999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>4</v>
       </c>
@@ -2109,8 +2331,11 @@
       <c r="F77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>252.178</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>4</v>
       </c>
@@ -2128,8 +2353,11 @@
       <c r="E78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78">
+        <v>245.24299999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>4</v>
       </c>
@@ -2150,8 +2378,11 @@
       <c r="F79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79">
+        <v>211.89599999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>4</v>
       </c>
@@ -2169,8 +2400,11 @@
       <c r="E80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <v>219.11600000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>4</v>
       </c>
@@ -2188,8 +2422,11 @@
       <c r="E81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81">
+        <v>126.831</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>4</v>
       </c>
@@ -2210,8 +2447,11 @@
       <c r="F82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <v>242.11199999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>5</v>
       </c>
@@ -2232,8 +2472,11 @@
       <c r="F83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83">
+        <v>342.27199999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>5</v>
       </c>
@@ -2251,8 +2494,11 @@
       <c r="E84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84">
+        <v>240.197</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>5</v>
       </c>
@@ -2273,8 +2519,11 @@
       <c r="F85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85">
+        <v>451.91500000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>5</v>
       </c>
@@ -2292,8 +2541,11 @@
       <c r="E86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86">
+        <v>309.03800000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>5</v>
       </c>
@@ -2314,8 +2566,11 @@
       <c r="F87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87">
+        <v>348.46899999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>5</v>
       </c>
@@ -2333,8 +2588,11 @@
       <c r="E88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88">
+        <v>409.86500000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>5</v>
       </c>
@@ -2355,8 +2613,11 @@
       <c r="F89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89">
+        <v>368.471</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>5</v>
       </c>
@@ -2374,8 +2635,11 @@
       <c r="E90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90">
+        <v>332.01600000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>5</v>
       </c>
@@ -2396,8 +2660,11 @@
       <c r="F91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91">
+        <v>249.69499999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>5</v>
       </c>
@@ -2415,8 +2682,11 @@
       <c r="E92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92">
+        <v>311.233</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>5</v>
       </c>
@@ -2434,8 +2704,11 @@
       <c r="E93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93">
+        <v>243.72499999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>5</v>
       </c>
@@ -2456,8 +2729,11 @@
       <c r="F94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94">
+        <v>335.22300000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>5</v>
       </c>
@@ -2478,8 +2754,11 @@
       <c r="F95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95">
+        <v>394.68400000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>5</v>
       </c>
@@ -2497,8 +2776,11 @@
       <c r="E96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G96">
+        <v>270.416</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>5</v>
       </c>
@@ -2516,8 +2798,11 @@
       <c r="E97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97">
+        <v>466.95600000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>5</v>
       </c>
@@ -2538,8 +2823,11 @@
       <c r="F98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G98">
+        <v>399.02499999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>5</v>
       </c>
@@ -2557,8 +2845,11 @@
       <c r="E99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G99">
+        <v>484.96300000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>5</v>
       </c>
@@ -2579,8 +2870,11 @@
       <c r="F100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G100">
+        <v>536.96600000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>5</v>
       </c>
@@ -2601,8 +2895,11 @@
       <c r="F101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G101">
+        <v>311.99700000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>5</v>
       </c>
@@ -2619,6 +2916,9 @@
       </c>
       <c r="E102">
         <v>1</v>
+      </c>
+      <c r="G102">
+        <v>451.31700000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spaghetti dataset added and tested with wandb.
Added extra documentation for some datasets
Created new algorithm for all networks
added new dataset spaghetti of all inserts
</commit_message>
<xml_diff>
--- a/code/Vision/Datasets/handmade/second_handmade/labels_new_bullet.xlsx
+++ b/code/Vision/Datasets/handmade/second_handmade/labels_new_bullet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsdepauw/Documents/Lars.nosync/Documents/School/1Ma ing/Masterproef/TWI/code/Vision/Datasets/handmade/second_handmade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B6E0B3-E6C4-5941-851C-08C6157C1A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2981D738-8741-6C44-9B6D-8F45DDD20491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{574AD3EE-55DF-7E4B-9902-E7692B0BE240}"/>
+    <workbookView xWindow="5960" yWindow="2140" windowWidth="27640" windowHeight="16940" xr2:uid="{574AD3EE-55DF-7E4B-9902-E7692B0BE240}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>img name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>stripe?</t>
   </si>
@@ -94,6 +91,15 @@
   <si>
     <t>Column14</t>
   </si>
+  <si>
+    <t>simgname</t>
+  </si>
+  <si>
+    <t>old_simgname</t>
+  </si>
+  <si>
+    <t>old_imgname</t>
+  </si>
 </sst>
 </file>
 
@@ -145,7 +151,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="000"/>
     </dxf>
@@ -172,9 +184,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82D6E0D0-B134-9D47-BD84-BCAE0931721B}" name="Table1" displayName="Table1" ref="A2:N102" totalsRowShown="0">
   <autoFilter ref="A2:N102" xr:uid="{D76D240F-1704-F54E-924C-7B401A31E2E8}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{3973C06F-4295-274C-8A0B-F470D90E49B7}" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{285FB392-8027-9048-9BA6-D360634C76DC}" name="Column2" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{79F4D1B8-0518-C142-AB57-020659483AD5}" name="Column3" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{3973C06F-4295-274C-8A0B-F470D90E49B7}" name="Column1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{285FB392-8027-9048-9BA6-D360634C76DC}" name="Column2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{79F4D1B8-0518-C142-AB57-020659483AD5}" name="Column3" dataDxfId="2">
       <calculatedColumnFormula>"b_"&amp;TEXT(A3,"000")&amp;"_p_"&amp;TEXT(B3,"000")&amp;IF(E3=1,"_s","_n")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{A44DD672-B998-1349-9CE0-020EA866E83D}" name="Column4">
@@ -184,8 +196,12 @@
     <tableColumn id="6" xr3:uid="{9755DD20-BD75-C348-95E0-07FD268BD674}" name="Column6"/>
     <tableColumn id="7" xr3:uid="{4F4F3C53-FD49-B34F-8EAD-384E284EBA38}" name="Column7"/>
     <tableColumn id="8" xr3:uid="{33C048BA-226E-BA45-B640-3FC2B232C56F}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{6CE7A930-4F20-D849-A9C2-03600EF6143F}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{1735DFDC-4727-B447-9379-B9ECC086E107}" name="Column10"/>
+    <tableColumn id="9" xr3:uid="{6CE7A930-4F20-D849-A9C2-03600EF6143F}" name="Column9" dataDxfId="1">
+      <calculatedColumnFormula>"b_"&amp;TEXT(A3,"000")&amp;"_p_"&amp;TEXT(B3,"000")&amp;IF(F3=1,"_b","_nb")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{1735DFDC-4727-B447-9379-B9ECC086E107}" name="Column10" dataDxfId="0">
+      <calculatedColumnFormula>"b_"&amp;TEXT(A3,"000")&amp;"_p_"&amp;TEXT(B3,"000")&amp;IF(F3=1,"_b","_nb")&amp;".jpg"</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="11" xr3:uid="{920FE2A5-1F5A-1941-9AAA-B07AB359B0D8}" name="Column11"/>
     <tableColumn id="12" xr3:uid="{0DD8F0C9-0CD1-444B-AE5E-9EE352B59E2E}" name="Column12"/>
     <tableColumn id="13" xr3:uid="{6EC5109A-C8C3-2844-BEF4-FF9371BFB78C}" name="Column13"/>
@@ -495,80 +511,88 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="10" max="14" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" customWidth="1"/>
+    <col min="10" max="10" width="37.5" customWidth="1"/>
+    <col min="11" max="14" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>18</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -592,6 +616,14 @@
       <c r="G3">
         <v>50.73</v>
       </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I34" si="0">"b_"&amp;TEXT(A3,"000")&amp;"_p_"&amp;TEXT(B3,"000")&amp;IF(F3=1,"_b","_nb")</f>
+        <v>b_001_p_001_nb</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J34" si="1">"b_"&amp;TEXT(A3,"000")&amp;"_p_"&amp;TEXT(B3,"000")&amp;IF(F3=1,"_b","_nb")&amp;".jpg"</f>
+        <v>b_001_p_001_nb.jpg</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -601,11 +633,11 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f t="shared" ref="C4:C67" si="0">"b_"&amp;TEXT(A4,"000")&amp;"_p_"&amp;TEXT(B4,"000")&amp;IF(E4=1,"_s","_n")</f>
+        <f t="shared" ref="C4:C67" si="2">"b_"&amp;TEXT(A4,"000")&amp;"_p_"&amp;TEXT(B4,"000")&amp;IF(E4=1,"_s","_n")</f>
         <v>b_001_p_001_s</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D67" si="1">"b_"&amp;TEXT(A4,"000")&amp;"_p_"&amp;TEXT(B4,"000")&amp;IF(E4=1,"_s","_n")&amp;".jpg"</f>
+        <f t="shared" ref="D4:D67" si="3">"b_"&amp;TEXT(A4,"000")&amp;"_p_"&amp;TEXT(B4,"000")&amp;IF(E4=1,"_s","_n")&amp;".jpg"</f>
         <v>b_001_p_001_s.jpg</v>
       </c>
       <c r="E4">
@@ -617,6 +649,14 @@
       <c r="G4">
         <v>57.122</v>
       </c>
+      <c r="I4" t="str">
+        <f>"b_"&amp;TEXT(A4,"000")&amp;"_p_"&amp;TEXT(B4,"000")&amp;IF(F4=1,"_b","_nb")</f>
+        <v>b_001_p_001_b</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_001_b.jpg</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -626,11 +666,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_002_n</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_002_n.jpg</v>
       </c>
       <c r="E5">
@@ -639,6 +679,14 @@
       <c r="G5">
         <v>46.984999999999999</v>
       </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_002_nb</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_002_nb.jpg</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -648,11 +696,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_002_s</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_002_s.jpg</v>
       </c>
       <c r="E6">
@@ -664,6 +712,14 @@
       <c r="G6">
         <v>68.903999999999996</v>
       </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_002_b</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_002_b.jpg</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -673,11 +729,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_003_n</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_003_n.jpg</v>
       </c>
       <c r="E7">
@@ -689,6 +745,14 @@
       <c r="G7">
         <v>35.348999999999997</v>
       </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_003_b</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_003_b.jpg</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -698,11 +762,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_003_s</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_003_s.jpg</v>
       </c>
       <c r="E8">
@@ -711,6 +775,14 @@
       <c r="G8">
         <v>32.594000000000001</v>
       </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_003_nb</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_003_nb.jpg</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -720,11 +792,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_004_n</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_004_n.jpg</v>
       </c>
       <c r="E9">
@@ -736,6 +808,14 @@
       <c r="G9">
         <v>38.79</v>
       </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_004_b</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_004_b.jpg</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -745,11 +825,11 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_004_s</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_004_s.jpg</v>
       </c>
       <c r="E10">
@@ -758,6 +838,14 @@
       <c r="G10">
         <v>47.353999999999999</v>
       </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_004_nb</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_004_nb.jpg</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -767,11 +855,11 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_005_n</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_005_n.jpg</v>
       </c>
       <c r="E11">
@@ -780,6 +868,14 @@
       <c r="G11">
         <v>42.637</v>
       </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_005_nb</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_005_nb.jpg</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -789,11 +885,11 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_005_s</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_005_s.jpg</v>
       </c>
       <c r="E12">
@@ -805,6 +901,14 @@
       <c r="G12">
         <v>44.158999999999999</v>
       </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_005_b</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_005_b.jpg</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -814,11 +918,11 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_006_n</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_006_n.jpg</v>
       </c>
       <c r="E13">
@@ -827,6 +931,14 @@
       <c r="G13">
         <v>40.957999999999998</v>
       </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_006_nb</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_006_nb.jpg</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -836,11 +948,11 @@
         <v>6.2727272727272698</v>
       </c>
       <c r="C14" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_006_s</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_006_s.jpg</v>
       </c>
       <c r="E14">
@@ -852,6 +964,14 @@
       <c r="G14">
         <v>40.505000000000003</v>
       </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_006_b</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_006_b.jpg</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -861,11 +981,11 @@
         <v>6.7727272727272698</v>
       </c>
       <c r="C15" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_007_n</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_007_n.jpg</v>
       </c>
       <c r="E15">
@@ -877,6 +997,14 @@
       <c r="G15">
         <v>34.71</v>
       </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_007_b</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_007_b.jpg</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -886,11 +1014,11 @@
         <v>7.2727272727272698</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_007_s</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_007_s.jpg</v>
       </c>
       <c r="E16">
@@ -899,8 +1027,16 @@
       <c r="G16">
         <v>44.46</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_007_nb</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_007_nb.jpg</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -908,11 +1044,11 @@
         <v>7.7727272727272698</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_008_n</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_008_n.jpg</v>
       </c>
       <c r="E17">
@@ -924,8 +1060,16 @@
       <c r="G17">
         <v>75.510000000000005</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_008_b</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_008_b.jpg</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -933,11 +1077,11 @@
         <v>8.2727272727272698</v>
       </c>
       <c r="C18" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_008_s</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_008_s.jpg</v>
       </c>
       <c r="E18">
@@ -946,8 +1090,16 @@
       <c r="G18">
         <v>37.774999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_008_nb</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_008_nb.jpg</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -955,11 +1107,11 @@
         <v>8.7727272727272698</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_009_n</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_009_n.jpg</v>
       </c>
       <c r="E19">
@@ -971,8 +1123,16 @@
       <c r="G19">
         <v>39.883000000000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_009_b</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_009_b.jpg</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -980,11 +1140,11 @@
         <v>9.2727272727272698</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_009_s</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_009_s.jpg</v>
       </c>
       <c r="E20">
@@ -993,8 +1153,16 @@
       <c r="G20">
         <v>53.984000000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_009_nb</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_009_nb.jpg</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1002,11 +1170,11 @@
         <v>9.7727272727272698</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_010_n</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_010_n.jpg</v>
       </c>
       <c r="E21">
@@ -1018,8 +1186,16 @@
       <c r="G21">
         <v>43.45</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_010_b</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_010_b.jpg</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1027,11 +1203,11 @@
         <v>10.2727272727273</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_001_p_010_s</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_001_p_010_s.jpg</v>
       </c>
       <c r="E22">
@@ -1040,8 +1216,16 @@
       <c r="G22">
         <v>51.164000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>b_001_p_010_nb</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v>b_001_p_010_nb.jpg</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -1049,11 +1233,11 @@
         <v>1</v>
       </c>
       <c r="C23" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_001_n</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_001_n.jpg</v>
       </c>
       <c r="E23">
@@ -1065,8 +1249,16 @@
       <c r="G23">
         <v>44.768999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_001_b</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_001_b.jpg</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1074,11 +1266,11 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_001_s</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_001_s.jpg</v>
       </c>
       <c r="E24">
@@ -1087,8 +1279,16 @@
       <c r="G24">
         <v>55.622</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_001_nb</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_001_nb.jpg</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -1096,11 +1296,11 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_002_n</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_002_n.jpg</v>
       </c>
       <c r="E25">
@@ -1112,8 +1312,16 @@
       <c r="G25">
         <v>55.427999999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_002_b</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_002_b.jpg</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -1121,11 +1329,11 @@
         <v>2</v>
       </c>
       <c r="C26" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_002_s</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_002_s.jpg</v>
       </c>
       <c r="E26">
@@ -1134,8 +1342,16 @@
       <c r="G26">
         <v>46.991</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_002_nb</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_002_nb.jpg</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -1143,11 +1359,11 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_003_n</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_003_n.jpg</v>
       </c>
       <c r="E27">
@@ -1159,8 +1375,16 @@
       <c r="G27">
         <v>32.549999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_003_b</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_003_b.jpg</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1168,11 +1392,11 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_003_s</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_003_s.jpg</v>
       </c>
       <c r="E28">
@@ -1181,8 +1405,16 @@
       <c r="G28">
         <v>40.301000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_003_nb</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_003_nb.jpg</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -1190,11 +1422,11 @@
         <v>4</v>
       </c>
       <c r="C29" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_004_n</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_004_n.jpg</v>
       </c>
       <c r="E29">
@@ -1203,8 +1435,16 @@
       <c r="G29">
         <v>27.945</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_004_nb</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_004_nb.jpg</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -1212,11 +1452,11 @@
         <v>4</v>
       </c>
       <c r="C30" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_004_s</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_004_s.jpg</v>
       </c>
       <c r="E30">
@@ -1228,8 +1468,16 @@
       <c r="G30">
         <v>31.759</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_004_b</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_004_b.jpg</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -1237,11 +1485,11 @@
         <v>5</v>
       </c>
       <c r="C31" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_005_n</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_005_n.jpg</v>
       </c>
       <c r="E31">
@@ -1250,8 +1498,16 @@
       <c r="G31">
         <v>44.09</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_005_nb</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_005_nb.jpg</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2</v>
       </c>
@@ -1259,11 +1515,11 @@
         <v>5</v>
       </c>
       <c r="C32" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_005_s</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_005_s.jpg</v>
       </c>
       <c r="E32">
@@ -1275,8 +1531,16 @@
       <c r="G32">
         <v>41.805</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_005_b</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_005_b.jpg</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2</v>
       </c>
@@ -1284,11 +1548,11 @@
         <v>6</v>
       </c>
       <c r="C33" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_006_n</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_006_n.jpg</v>
       </c>
       <c r="E33">
@@ -1300,8 +1564,16 @@
       <c r="G33">
         <v>54.143999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_006_b</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_006_b.jpg</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -1309,11 +1581,11 @@
         <v>6.2727272727272698</v>
       </c>
       <c r="C34" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_006_s</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_006_s.jpg</v>
       </c>
       <c r="E34">
@@ -1322,8 +1594,16 @@
       <c r="G34">
         <v>42.021999999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>b_002_p_006_nb</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="1"/>
+        <v>b_002_p_006_nb.jpg</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2</v>
       </c>
@@ -1331,11 +1611,11 @@
         <v>6.7727272727272698</v>
       </c>
       <c r="C35" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_007_n</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_007_n.jpg</v>
       </c>
       <c r="E35">
@@ -1344,8 +1624,16 @@
       <c r="G35">
         <v>70.105000000000004</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I35" t="str">
+        <f t="shared" ref="I35:I66" si="4">"b_"&amp;TEXT(A35,"000")&amp;"_p_"&amp;TEXT(B35,"000")&amp;IF(F35=1,"_b","_nb")</f>
+        <v>b_002_p_007_nb</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" ref="J35:J66" si="5">"b_"&amp;TEXT(A35,"000")&amp;"_p_"&amp;TEXT(B35,"000")&amp;IF(F35=1,"_b","_nb")&amp;".jpg"</f>
+        <v>b_002_p_007_nb.jpg</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -1353,11 +1641,11 @@
         <v>7.2727272727272698</v>
       </c>
       <c r="C36" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_007_s</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_007_s.jpg</v>
       </c>
       <c r="E36">
@@ -1369,8 +1657,16 @@
       <c r="G36">
         <v>76.501999999999995</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I36" t="str">
+        <f t="shared" si="4"/>
+        <v>b_002_p_007_b</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="5"/>
+        <v>b_002_p_007_b.jpg</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -1378,11 +1674,11 @@
         <v>7.7727272727272698</v>
       </c>
       <c r="C37" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_008_n</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_008_n.jpg</v>
       </c>
       <c r="E37">
@@ -1394,8 +1690,16 @@
       <c r="G37">
         <v>58.457000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I37" t="str">
+        <f t="shared" si="4"/>
+        <v>b_002_p_008_b</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="5"/>
+        <v>b_002_p_008_b.jpg</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2</v>
       </c>
@@ -1403,11 +1707,11 @@
         <v>8.2727272727272698</v>
       </c>
       <c r="C38" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_008_s</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_008_s.jpg</v>
       </c>
       <c r="E38">
@@ -1416,8 +1720,16 @@
       <c r="G38">
         <v>72.137</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I38" t="str">
+        <f t="shared" si="4"/>
+        <v>b_002_p_008_nb</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="5"/>
+        <v>b_002_p_008_nb.jpg</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -1425,11 +1737,11 @@
         <v>8.7727272727272698</v>
       </c>
       <c r="C39" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_009_n</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_009_n.jpg</v>
       </c>
       <c r="E39">
@@ -1438,8 +1750,16 @@
       <c r="G39">
         <v>108.938</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I39" t="str">
+        <f t="shared" si="4"/>
+        <v>b_002_p_009_nb</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="5"/>
+        <v>b_002_p_009_nb.jpg</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -1447,11 +1767,11 @@
         <v>9.2727272727272698</v>
       </c>
       <c r="C40" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_009_s</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_009_s.jpg</v>
       </c>
       <c r="E40">
@@ -1463,8 +1783,16 @@
       <c r="G40">
         <v>136.44200000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I40" t="str">
+        <f t="shared" si="4"/>
+        <v>b_002_p_009_b</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="5"/>
+        <v>b_002_p_009_b.jpg</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -1472,11 +1800,11 @@
         <v>9.7727272727272698</v>
       </c>
       <c r="C41" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_010_n</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_010_n.jpg</v>
       </c>
       <c r="E41">
@@ -1485,8 +1813,16 @@
       <c r="G41">
         <v>114.246</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I41" t="str">
+        <f t="shared" si="4"/>
+        <v>b_002_p_010_nb</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="5"/>
+        <v>b_002_p_010_nb.jpg</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -1494,11 +1830,11 @@
         <v>10.2727272727273</v>
       </c>
       <c r="C42" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_002_p_010_s</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_002_p_010_s.jpg</v>
       </c>
       <c r="E42">
@@ -1510,8 +1846,16 @@
       <c r="G42">
         <v>69.489999999999995</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I42" t="str">
+        <f t="shared" si="4"/>
+        <v>b_002_p_010_b</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="5"/>
+        <v>b_002_p_010_b.jpg</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>3</v>
       </c>
@@ -1519,11 +1863,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_001_n</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_001_n.jpg</v>
       </c>
       <c r="E43">
@@ -1535,8 +1879,16 @@
       <c r="G43">
         <v>157.529</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I43" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_001_b</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_001_b.jpg</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>3</v>
       </c>
@@ -1544,11 +1896,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_001_s</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_001_s.jpg</v>
       </c>
       <c r="E44">
@@ -1557,8 +1909,16 @@
       <c r="G44">
         <v>150.964</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I44" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_001_nb</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_001_nb.jpg</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -1566,11 +1926,11 @@
         <v>2</v>
       </c>
       <c r="C45" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_002_n</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_002_n.jpg</v>
       </c>
       <c r="E45">
@@ -1579,8 +1939,16 @@
       <c r="G45">
         <v>163.71</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I45" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_002_nb</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_002_nb.jpg</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>3</v>
       </c>
@@ -1588,11 +1956,11 @@
         <v>2</v>
       </c>
       <c r="C46" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_002_s</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_002_s.jpg</v>
       </c>
       <c r="E46">
@@ -1604,8 +1972,16 @@
       <c r="G46">
         <v>250.45099999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I46" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_002_b</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_002_b.jpg</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>3</v>
       </c>
@@ -1613,11 +1989,11 @@
         <v>3</v>
       </c>
       <c r="C47" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_003_n</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_003_n.jpg</v>
       </c>
       <c r="E47">
@@ -1626,8 +2002,16 @@
       <c r="G47">
         <v>176.70699999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I47" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_003_nb</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_003_nb.jpg</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>3</v>
       </c>
@@ -1635,11 +2019,11 @@
         <v>3</v>
       </c>
       <c r="C48" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_003_s</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_003_s.jpg</v>
       </c>
       <c r="E48">
@@ -1651,8 +2035,16 @@
       <c r="G48">
         <v>272.12599999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I48" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_003_b</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_003_b.jpg</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -1660,11 +2052,11 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_004_n</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_004_n.jpg</v>
       </c>
       <c r="E49">
@@ -1673,8 +2065,16 @@
       <c r="G49">
         <v>159.685</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I49" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_004_nb</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_004_nb.jpg</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>3</v>
       </c>
@@ -1682,11 +2082,11 @@
         <v>4</v>
       </c>
       <c r="C50" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_004_s</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_004_s.jpg</v>
       </c>
       <c r="E50">
@@ -1698,8 +2098,16 @@
       <c r="G50">
         <v>262.48700000000002</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I50" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_004_b</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_004_b.jpg</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>3</v>
       </c>
@@ -1707,11 +2115,11 @@
         <v>5</v>
       </c>
       <c r="C51" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_005_n</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_005_n.jpg</v>
       </c>
       <c r="E51">
@@ -1720,8 +2128,16 @@
       <c r="G51">
         <v>202.03200000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I51" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_005_nb</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_005_nb.jpg</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>3</v>
       </c>
@@ -1729,11 +2145,11 @@
         <v>5</v>
       </c>
       <c r="C52" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_005_s</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_005_s.jpg</v>
       </c>
       <c r="E52">
@@ -1745,8 +2161,16 @@
       <c r="G52">
         <v>161.91300000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I52" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_005_b</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_005_b.jpg</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>3</v>
       </c>
@@ -1754,11 +2178,11 @@
         <v>6</v>
       </c>
       <c r="C53" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_006_n</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_006_n.jpg</v>
       </c>
       <c r="E53">
@@ -1770,8 +2194,16 @@
       <c r="G53">
         <v>389.15</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I53" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_006_b</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_006_b.jpg</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>3</v>
       </c>
@@ -1779,11 +2211,11 @@
         <v>6.2727272727272698</v>
       </c>
       <c r="C54" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_006_s</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_006_s.jpg</v>
       </c>
       <c r="E54">
@@ -1792,8 +2224,16 @@
       <c r="G54">
         <v>287.17</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I54" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_006_nb</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_006_nb.jpg</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -1801,11 +2241,11 @@
         <v>6.7727272727272698</v>
       </c>
       <c r="C55" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_007_n</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_007_n.jpg</v>
       </c>
       <c r="E55">
@@ -1814,8 +2254,16 @@
       <c r="G55">
         <v>172.22200000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I55" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_007_nb</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_007_nb.jpg</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>3</v>
       </c>
@@ -1823,11 +2271,11 @@
         <v>7.2727272727272698</v>
       </c>
       <c r="C56" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_007_s</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_007_s.jpg</v>
       </c>
       <c r="E56">
@@ -1839,8 +2287,16 @@
       <c r="G56">
         <v>143.72300000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I56" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_007_b</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_007_b.jpg</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>3</v>
       </c>
@@ -1848,11 +2304,11 @@
         <v>7.7727272727272698</v>
       </c>
       <c r="C57" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_008_n</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_008_n.jpg</v>
       </c>
       <c r="E57">
@@ -1864,8 +2320,16 @@
       <c r="G57">
         <v>162.71199999999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I57" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_008_b</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_008_b.jpg</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>3</v>
       </c>
@@ -1873,11 +2337,11 @@
         <v>8.2727272727272698</v>
       </c>
       <c r="C58" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_008_s</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_008_s.jpg</v>
       </c>
       <c r="E58">
@@ -1886,8 +2350,16 @@
       <c r="G58">
         <v>147.59100000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I58" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_008_nb</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_008_nb.jpg</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -1895,11 +2367,11 @@
         <v>8.7727272727272698</v>
       </c>
       <c r="C59" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_009_n</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_009_n.jpg</v>
       </c>
       <c r="E59">
@@ -1908,8 +2380,16 @@
       <c r="G59">
         <v>177.483</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I59" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_009_nb</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_009_nb.jpg</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>3</v>
       </c>
@@ -1917,11 +2397,11 @@
         <v>9.2727272727272698</v>
       </c>
       <c r="C60" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_009_s</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_009_s.jpg</v>
       </c>
       <c r="E60">
@@ -1933,8 +2413,16 @@
       <c r="G60">
         <v>141.84</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I60" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_009_b</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_009_b.jpg</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>3</v>
       </c>
@@ -1942,11 +2430,11 @@
         <v>9.7727272727272698</v>
       </c>
       <c r="C61" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_010_n</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_010_n.jpg</v>
       </c>
       <c r="E61">
@@ -1955,8 +2443,16 @@
       <c r="G61">
         <v>168.27199999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I61" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_010_nb</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_010_nb.jpg</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>3</v>
       </c>
@@ -1964,11 +2460,11 @@
         <v>10.2727272727273</v>
       </c>
       <c r="C62" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_003_p_010_s</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_003_p_010_s.jpg</v>
       </c>
       <c r="E62">
@@ -1980,8 +2476,16 @@
       <c r="G62">
         <v>164.79</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I62" t="str">
+        <f t="shared" si="4"/>
+        <v>b_003_p_010_b</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="5"/>
+        <v>b_003_p_010_b.jpg</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>4</v>
       </c>
@@ -1989,11 +2493,11 @@
         <v>1</v>
       </c>
       <c r="C63" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_004_p_001_n</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_004_p_001_n.jpg</v>
       </c>
       <c r="E63">
@@ -2002,8 +2506,16 @@
       <c r="G63">
         <v>170.90299999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I63" t="str">
+        <f t="shared" si="4"/>
+        <v>b_004_p_001_nb</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="5"/>
+        <v>b_004_p_001_nb.jpg</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>4</v>
       </c>
@@ -2011,11 +2523,11 @@
         <v>1</v>
       </c>
       <c r="C64" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_004_p_001_s</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_004_p_001_s.jpg</v>
       </c>
       <c r="E64">
@@ -2027,8 +2539,16 @@
       <c r="G64">
         <v>194.83199999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I64" t="str">
+        <f t="shared" si="4"/>
+        <v>b_004_p_001_b</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="5"/>
+        <v>b_004_p_001_b.jpg</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>4</v>
       </c>
@@ -2036,11 +2556,11 @@
         <v>2</v>
       </c>
       <c r="C65" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_004_p_002_n</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_004_p_002_n.jpg</v>
       </c>
       <c r="E65">
@@ -2049,8 +2569,16 @@
       <c r="G65">
         <v>236.77699999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I65" t="str">
+        <f t="shared" si="4"/>
+        <v>b_004_p_002_nb</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="5"/>
+        <v>b_004_p_002_nb.jpg</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>4</v>
       </c>
@@ -2058,11 +2586,11 @@
         <v>2</v>
       </c>
       <c r="C66" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_004_p_002_s</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_004_p_002_s.jpg</v>
       </c>
       <c r="E66">
@@ -2074,8 +2602,16 @@
       <c r="G66">
         <v>279.31799999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I66" t="str">
+        <f t="shared" si="4"/>
+        <v>b_004_p_002_b</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="5"/>
+        <v>b_004_p_002_b.jpg</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>4</v>
       </c>
@@ -2083,11 +2619,11 @@
         <v>3</v>
       </c>
       <c r="C67" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>b_004_p_003_n</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>b_004_p_003_n.jpg</v>
       </c>
       <c r="E67">
@@ -2099,8 +2635,16 @@
       <c r="G67">
         <v>234.07400000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I67" t="str">
+        <f t="shared" ref="I67:I102" si="6">"b_"&amp;TEXT(A67,"000")&amp;"_p_"&amp;TEXT(B67,"000")&amp;IF(F67=1,"_b","_nb")</f>
+        <v>b_004_p_003_b</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J102" si="7">"b_"&amp;TEXT(A67,"000")&amp;"_p_"&amp;TEXT(B67,"000")&amp;IF(F67=1,"_b","_nb")&amp;".jpg"</f>
+        <v>b_004_p_003_b.jpg</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>4</v>
       </c>
@@ -2108,11 +2652,11 @@
         <v>3</v>
       </c>
       <c r="C68" s="2" t="str">
-        <f t="shared" ref="C68:C102" si="2">"b_"&amp;TEXT(A68,"000")&amp;"_p_"&amp;TEXT(B68,"000")&amp;IF(E68=1,"_s","_n")</f>
+        <f t="shared" ref="C68:C102" si="8">"b_"&amp;TEXT(A68,"000")&amp;"_p_"&amp;TEXT(B68,"000")&amp;IF(E68=1,"_s","_n")</f>
         <v>b_004_p_003_s</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" ref="D68:D102" si="3">"b_"&amp;TEXT(A68,"000")&amp;"_p_"&amp;TEXT(B68,"000")&amp;IF(E68=1,"_s","_n")&amp;".jpg"</f>
+        <f t="shared" ref="D68:D102" si="9">"b_"&amp;TEXT(A68,"000")&amp;"_p_"&amp;TEXT(B68,"000")&amp;IF(E68=1,"_s","_n")&amp;".jpg"</f>
         <v>b_004_p_003_s.jpg</v>
       </c>
       <c r="E68">
@@ -2121,8 +2665,16 @@
       <c r="G68">
         <v>212.64400000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I68" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_003_nb</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_003_nb.jpg</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>4</v>
       </c>
@@ -2130,11 +2682,11 @@
         <v>4</v>
       </c>
       <c r="C69" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_004_n</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_004_n.jpg</v>
       </c>
       <c r="E69">
@@ -2143,8 +2695,16 @@
       <c r="G69">
         <v>321.149</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I69" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_004_nb</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_004_nb.jpg</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>4</v>
       </c>
@@ -2152,11 +2712,11 @@
         <v>4</v>
       </c>
       <c r="C70" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_004_s</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_004_s.jpg</v>
       </c>
       <c r="E70">
@@ -2168,8 +2728,16 @@
       <c r="G70">
         <v>226.673</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I70" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_004_b</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_004_b.jpg</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>4</v>
       </c>
@@ -2177,11 +2745,11 @@
         <v>5</v>
       </c>
       <c r="C71" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_005_n</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_005_n.jpg</v>
       </c>
       <c r="E71">
@@ -2190,8 +2758,16 @@
       <c r="G71">
         <v>268.22699999999998</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I71" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_005_nb</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_005_nb.jpg</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>4</v>
       </c>
@@ -2199,11 +2775,11 @@
         <v>5</v>
       </c>
       <c r="C72" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_005_s</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_005_s.jpg</v>
       </c>
       <c r="E72">
@@ -2215,8 +2791,16 @@
       <c r="G72">
         <v>250.97900000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I72" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_005_b</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_005_b.jpg</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>4</v>
       </c>
@@ -2224,11 +2808,11 @@
         <v>6</v>
       </c>
       <c r="C73" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_006_n</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_006_n.jpg</v>
       </c>
       <c r="E73">
@@ -2240,8 +2824,16 @@
       <c r="G73">
         <v>157.04</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I73" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_006_b</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_006_b.jpg</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>4</v>
       </c>
@@ -2249,11 +2841,11 @@
         <v>6.2727272727272698</v>
       </c>
       <c r="C74" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_006_s</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_006_s.jpg</v>
       </c>
       <c r="E74">
@@ -2262,8 +2854,16 @@
       <c r="G74">
         <v>227.3</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I74" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_006_nb</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_006_nb.jpg</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>4</v>
       </c>
@@ -2271,11 +2871,11 @@
         <v>6.7727272727272698</v>
       </c>
       <c r="C75" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_007_n</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_007_n.jpg</v>
       </c>
       <c r="E75">
@@ -2284,8 +2884,16 @@
       <c r="G75">
         <v>180.68799999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I75" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_007_nb</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_007_nb.jpg</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>4</v>
       </c>
@@ -2293,11 +2901,11 @@
         <v>7.2727272727272698</v>
       </c>
       <c r="C76" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_007_s</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_007_s.jpg</v>
       </c>
       <c r="E76">
@@ -2309,8 +2917,16 @@
       <c r="G76">
         <v>192.24799999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I76" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_007_b</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_007_b.jpg</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>4</v>
       </c>
@@ -2318,11 +2934,11 @@
         <v>7.7727272727272698</v>
       </c>
       <c r="C77" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_008_n</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_008_n.jpg</v>
       </c>
       <c r="E77">
@@ -2334,8 +2950,16 @@
       <c r="G77">
         <v>252.178</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I77" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_008_b</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_008_b.jpg</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>4</v>
       </c>
@@ -2343,11 +2967,11 @@
         <v>8.2727272727272698</v>
       </c>
       <c r="C78" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_008_s</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_008_s.jpg</v>
       </c>
       <c r="E78">
@@ -2356,8 +2980,16 @@
       <c r="G78">
         <v>245.24299999999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I78" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_008_nb</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_008_nb.jpg</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>4</v>
       </c>
@@ -2365,11 +2997,11 @@
         <v>8.7727272727272698</v>
       </c>
       <c r="C79" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_009_n</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_009_n.jpg</v>
       </c>
       <c r="E79">
@@ -2381,8 +3013,16 @@
       <c r="G79">
         <v>211.89599999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I79" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_009_b</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_009_b.jpg</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>4</v>
       </c>
@@ -2390,11 +3030,11 @@
         <v>9.2727272727272698</v>
       </c>
       <c r="C80" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_009_s</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_009_s.jpg</v>
       </c>
       <c r="E80">
@@ -2403,8 +3043,16 @@
       <c r="G80">
         <v>219.11600000000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I80" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_009_nb</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_009_nb.jpg</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>4</v>
       </c>
@@ -2412,11 +3060,11 @@
         <v>9.7727272727272698</v>
       </c>
       <c r="C81" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_010_n</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_010_n.jpg</v>
       </c>
       <c r="E81">
@@ -2425,8 +3073,16 @@
       <c r="G81">
         <v>126.831</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I81" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_010_nb</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_010_nb.jpg</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>4</v>
       </c>
@@ -2434,11 +3090,11 @@
         <v>10.2727272727273</v>
       </c>
       <c r="C82" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_004_p_010_s</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_004_p_010_s.jpg</v>
       </c>
       <c r="E82">
@@ -2450,8 +3106,16 @@
       <c r="G82">
         <v>242.11199999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I82" t="str">
+        <f t="shared" si="6"/>
+        <v>b_004_p_010_b</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="7"/>
+        <v>b_004_p_010_b.jpg</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>5</v>
       </c>
@@ -2459,11 +3123,11 @@
         <v>1</v>
       </c>
       <c r="C83" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_001_n</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_001_n.jpg</v>
       </c>
       <c r="E83">
@@ -2475,8 +3139,16 @@
       <c r="G83">
         <v>342.27199999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I83" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_001_b</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_001_b.jpg</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>5</v>
       </c>
@@ -2484,11 +3156,11 @@
         <v>1</v>
       </c>
       <c r="C84" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_001_s</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_001_s.jpg</v>
       </c>
       <c r="E84">
@@ -2497,8 +3169,16 @@
       <c r="G84">
         <v>240.197</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I84" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_001_nb</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_001_nb.jpg</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>5</v>
       </c>
@@ -2506,11 +3186,11 @@
         <v>2</v>
       </c>
       <c r="C85" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_002_n</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_002_n.jpg</v>
       </c>
       <c r="E85">
@@ -2522,8 +3202,16 @@
       <c r="G85">
         <v>451.91500000000002</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I85" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_002_b</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_002_b.jpg</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>5</v>
       </c>
@@ -2531,11 +3219,11 @@
         <v>2</v>
       </c>
       <c r="C86" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_002_s</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_002_s.jpg</v>
       </c>
       <c r="E86">
@@ -2544,8 +3232,16 @@
       <c r="G86">
         <v>309.03800000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I86" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_002_nb</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_002_nb.jpg</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>5</v>
       </c>
@@ -2553,11 +3249,11 @@
         <v>3</v>
       </c>
       <c r="C87" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_003_n</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_003_n.jpg</v>
       </c>
       <c r="E87">
@@ -2569,8 +3265,16 @@
       <c r="G87">
         <v>348.46899999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I87" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_003_b</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_003_b.jpg</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>5</v>
       </c>
@@ -2578,11 +3282,11 @@
         <v>3</v>
       </c>
       <c r="C88" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_003_s</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_003_s.jpg</v>
       </c>
       <c r="E88">
@@ -2591,8 +3295,16 @@
       <c r="G88">
         <v>409.86500000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I88" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_003_nb</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_003_nb.jpg</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>5</v>
       </c>
@@ -2600,11 +3312,11 @@
         <v>4</v>
       </c>
       <c r="C89" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_004_n</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_004_n.jpg</v>
       </c>
       <c r="E89">
@@ -2616,8 +3328,16 @@
       <c r="G89">
         <v>368.471</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I89" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_004_b</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_004_b.jpg</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>5</v>
       </c>
@@ -2625,11 +3345,11 @@
         <v>4</v>
       </c>
       <c r="C90" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_004_s</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_004_s.jpg</v>
       </c>
       <c r="E90">
@@ -2638,8 +3358,16 @@
       <c r="G90">
         <v>332.01600000000002</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I90" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_004_nb</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_004_nb.jpg</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>5</v>
       </c>
@@ -2647,11 +3375,11 @@
         <v>5</v>
       </c>
       <c r="C91" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_005_n</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_005_n.jpg</v>
       </c>
       <c r="E91">
@@ -2663,8 +3391,16 @@
       <c r="G91">
         <v>249.69499999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I91" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_005_b</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_005_b.jpg</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>5</v>
       </c>
@@ -2672,11 +3408,11 @@
         <v>5</v>
       </c>
       <c r="C92" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_005_s</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_005_s.jpg</v>
       </c>
       <c r="E92">
@@ -2685,8 +3421,16 @@
       <c r="G92">
         <v>311.233</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I92" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_005_nb</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_005_nb.jpg</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>5</v>
       </c>
@@ -2694,11 +3438,11 @@
         <v>6</v>
       </c>
       <c r="C93" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_006_n</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_006_n.jpg</v>
       </c>
       <c r="E93">
@@ -2707,8 +3451,16 @@
       <c r="G93">
         <v>243.72499999999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I93" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_006_nb</v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_006_nb.jpg</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>5</v>
       </c>
@@ -2716,11 +3468,11 @@
         <v>6.2727272727272698</v>
       </c>
       <c r="C94" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_006_s</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_006_s.jpg</v>
       </c>
       <c r="E94">
@@ -2732,8 +3484,16 @@
       <c r="G94">
         <v>335.22300000000001</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I94" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_006_b</v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_006_b.jpg</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>5</v>
       </c>
@@ -2741,11 +3501,11 @@
         <v>6.7727272727272698</v>
       </c>
       <c r="C95" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_007_n</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_007_n.jpg</v>
       </c>
       <c r="E95">
@@ -2757,8 +3517,16 @@
       <c r="G95">
         <v>394.68400000000003</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I95" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_007_b</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_007_b.jpg</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>5</v>
       </c>
@@ -2766,11 +3534,11 @@
         <v>7.2727272727272698</v>
       </c>
       <c r="C96" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_007_s</v>
       </c>
       <c r="D96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_007_s.jpg</v>
       </c>
       <c r="E96">
@@ -2779,8 +3547,16 @@
       <c r="G96">
         <v>270.416</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I96" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_007_nb</v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_007_nb.jpg</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>5</v>
       </c>
@@ -2788,11 +3564,11 @@
         <v>7.7727272727272698</v>
       </c>
       <c r="C97" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_008_n</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_008_n.jpg</v>
       </c>
       <c r="E97">
@@ -2801,8 +3577,16 @@
       <c r="G97">
         <v>466.95600000000002</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I97" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_008_nb</v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_008_nb.jpg</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>5</v>
       </c>
@@ -2810,11 +3594,11 @@
         <v>8.2727272727272698</v>
       </c>
       <c r="C98" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_008_s</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_008_s.jpg</v>
       </c>
       <c r="E98">
@@ -2826,8 +3610,16 @@
       <c r="G98">
         <v>399.02499999999998</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I98" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_008_b</v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_008_b.jpg</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>5</v>
       </c>
@@ -2835,11 +3627,11 @@
         <v>8.7727272727272698</v>
       </c>
       <c r="C99" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_009_n</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_009_n.jpg</v>
       </c>
       <c r="E99">
@@ -2848,8 +3640,16 @@
       <c r="G99">
         <v>484.96300000000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I99" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_009_nb</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_009_nb.jpg</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>5</v>
       </c>
@@ -2857,11 +3657,11 @@
         <v>9.2727272727272698</v>
       </c>
       <c r="C100" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_009_s</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_009_s.jpg</v>
       </c>
       <c r="E100">
@@ -2873,8 +3673,16 @@
       <c r="G100">
         <v>536.96600000000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I100" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_009_b</v>
+      </c>
+      <c r="J100" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_009_b.jpg</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>5</v>
       </c>
@@ -2882,11 +3690,11 @@
         <v>9.7727272727272698</v>
       </c>
       <c r="C101" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_010_n</v>
       </c>
       <c r="D101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_010_n.jpg</v>
       </c>
       <c r="E101">
@@ -2898,8 +3706,16 @@
       <c r="G101">
         <v>311.99700000000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I101" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_010_b</v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_010_b.jpg</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>5</v>
       </c>
@@ -2907,11 +3723,11 @@
         <v>10.2727272727273</v>
       </c>
       <c r="C102" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>b_005_p_010_s</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>b_005_p_010_s.jpg</v>
       </c>
       <c r="E102">
@@ -2920,9 +3736,18 @@
       <c r="G102">
         <v>451.31700000000001</v>
       </c>
+      <c r="I102" t="str">
+        <f t="shared" si="6"/>
+        <v>b_005_p_010_nb</v>
+      </c>
+      <c r="J102" t="str">
+        <f t="shared" si="7"/>
+        <v>b_005_p_010_nb.jpg</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>